<commit_message>
moving between menus and functions using json callbacks instead of the concatenation of the route - allowing to keep each users state in his session data structure. changing the menu logic due to the changes above.
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erantirer/PycharmProjects/PsychometricTestBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5842938F-14B5-AF41-B0B3-679489C51743}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707998B0-16E9-BB42-91FD-296B9AD986FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26565,7 +26565,9 @@
   <sheetPr codeName="גיליון1"/>
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>